<commit_message>
periodo de conciliación y ajuste rol de consulta inicio
</commit_message>
<xml_diff>
--- a/help/conciliacion_plantilla.xlsx
+++ b/help/conciliacion_plantilla.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26626"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B3F15E4-0470-40FE-B393-35A5719A8F30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56D471AF-E224-44B0-BD43-64BC2B7B509F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CONCILIACION" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="109">
   <si>
     <t>INSTITUTO NACIONAL DE VIAS
 SUBDIRECCION DE SOSTENIBILIAD Y GRUPO DE CONTABILIDAD
@@ -358,6 +358,9 @@
   </si>
   <si>
     <t>${G55}</t>
+  </si>
+  <si>
+    <t>${I4}</t>
   </si>
 </sst>
 </file>
@@ -1030,6 +1033,183 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="6" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="7" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="7" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1053,183 +1233,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="7" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="7" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="6" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1600,7 +1603,7 @@
   <dimension ref="B1:M82"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1623,13 +1626,13 @@
       <c r="B2" s="2"/>
       <c r="C2" s="3"/>
       <c r="D2" s="4"/>
-      <c r="E2" s="119" t="s">
+      <c r="E2" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="119"/>
-      <c r="G2" s="119"/>
-      <c r="H2" s="119"/>
-      <c r="I2" s="120"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="56"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="5"/>
@@ -1641,18 +1644,20 @@
     </row>
     <row r="4" spans="2:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="5"/>
-      <c r="D4" s="121" t="s">
+      <c r="D4" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="121"/>
+      <c r="E4" s="57"/>
       <c r="F4" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="G4" s="121" t="s">
+      <c r="G4" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="121"/>
-      <c r="I4" s="9"/>
+      <c r="H4" s="57"/>
+      <c r="I4" s="9" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="5"/>
@@ -1664,15 +1669,15 @@
     </row>
     <row r="6" spans="2:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="5"/>
-      <c r="D6" s="89" t="s">
+      <c r="D6" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="91"/>
+      <c r="E6" s="59"/>
       <c r="F6" s="11"/>
-      <c r="G6" s="89" t="s">
+      <c r="G6" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="91"/>
+      <c r="H6" s="59"/>
       <c r="I6" s="12"/>
     </row>
     <row r="7" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1712,16 +1717,16 @@
       <c r="I9" s="12"/>
     </row>
     <row r="10" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="86" t="s">
+      <c r="B10" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="87"/>
-      <c r="D10" s="87"/>
-      <c r="E10" s="87"/>
-      <c r="F10" s="87"/>
-      <c r="G10" s="87"/>
-      <c r="H10" s="87"/>
-      <c r="I10" s="88"/>
+      <c r="C10" s="61"/>
+      <c r="D10" s="61"/>
+      <c r="E10" s="61"/>
+      <c r="F10" s="61"/>
+      <c r="G10" s="61"/>
+      <c r="H10" s="61"/>
+      <c r="I10" s="62"/>
     </row>
     <row r="11" spans="2:9" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="2"/>
@@ -1735,68 +1740,68 @@
     </row>
     <row r="12" spans="2:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="5"/>
-      <c r="D12" s="89" t="s">
+      <c r="D12" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="91"/>
+      <c r="E12" s="59"/>
       <c r="F12" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="108" t="s">
+      <c r="G12" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="H12" s="109"/>
-      <c r="I12" s="110"/>
+      <c r="H12" s="64"/>
+      <c r="I12" s="65"/>
     </row>
     <row r="13" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="5"/>
-      <c r="D13" s="111" t="s">
+      <c r="D13" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="112"/>
-      <c r="F13" s="117">
+      <c r="E13" s="67"/>
+      <c r="F13" s="72">
         <f>SUM(G13:G33)</f>
         <v>0</v>
       </c>
       <c r="G13" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="H13" s="115" t="s">
+      <c r="H13" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="I13" s="116"/>
+      <c r="I13" s="71"/>
     </row>
     <row r="14" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="5"/>
-      <c r="D14" s="113"/>
-      <c r="E14" s="114"/>
-      <c r="F14" s="118"/>
+      <c r="D14" s="68"/>
+      <c r="E14" s="69"/>
+      <c r="F14" s="73"/>
       <c r="G14" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="H14" s="115" t="s">
+      <c r="H14" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="I14" s="116"/>
+      <c r="I14" s="71"/>
     </row>
     <row r="15" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="5"/>
-      <c r="D15" s="113"/>
-      <c r="E15" s="114"/>
-      <c r="F15" s="118"/>
+      <c r="D15" s="68"/>
+      <c r="E15" s="69"/>
+      <c r="F15" s="73"/>
       <c r="G15" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="H15" s="115" t="s">
+      <c r="H15" s="70" t="s">
         <v>16</v>
       </c>
-      <c r="I15" s="116"/>
+      <c r="I15" s="71"/>
     </row>
     <row r="16" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="5"/>
-      <c r="D16" s="113"/>
-      <c r="E16" s="114"/>
-      <c r="F16" s="118"/>
+      <c r="D16" s="68"/>
+      <c r="E16" s="69"/>
+      <c r="F16" s="73"/>
       <c r="G16" s="16" t="s">
         <v>74</v>
       </c>
@@ -1807,9 +1812,9 @@
     </row>
     <row r="17" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="5"/>
-      <c r="D17" s="113"/>
-      <c r="E17" s="114"/>
-      <c r="F17" s="118"/>
+      <c r="D17" s="68"/>
+      <c r="E17" s="69"/>
+      <c r="F17" s="73"/>
       <c r="G17" s="16" t="s">
         <v>75</v>
       </c>
@@ -1820,9 +1825,9 @@
     </row>
     <row r="18" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="5"/>
-      <c r="D18" s="113"/>
-      <c r="E18" s="114"/>
-      <c r="F18" s="118"/>
+      <c r="D18" s="68"/>
+      <c r="E18" s="69"/>
+      <c r="F18" s="73"/>
       <c r="G18" s="16" t="s">
         <v>76</v>
       </c>
@@ -1833,9 +1838,9 @@
     </row>
     <row r="19" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="5"/>
-      <c r="D19" s="113"/>
-      <c r="E19" s="114"/>
-      <c r="F19" s="118"/>
+      <c r="D19" s="68"/>
+      <c r="E19" s="69"/>
+      <c r="F19" s="73"/>
       <c r="G19" s="16" t="s">
         <v>77</v>
       </c>
@@ -1846,9 +1851,9 @@
     </row>
     <row r="20" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="5"/>
-      <c r="D20" s="113"/>
-      <c r="E20" s="114"/>
-      <c r="F20" s="118"/>
+      <c r="D20" s="68"/>
+      <c r="E20" s="69"/>
+      <c r="F20" s="73"/>
       <c r="G20" s="16" t="s">
         <v>78</v>
       </c>
@@ -1859,9 +1864,9 @@
     </row>
     <row r="21" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="5"/>
-      <c r="D21" s="113"/>
-      <c r="E21" s="114"/>
-      <c r="F21" s="118"/>
+      <c r="D21" s="68"/>
+      <c r="E21" s="69"/>
+      <c r="F21" s="73"/>
       <c r="G21" s="16" t="s">
         <v>79</v>
       </c>
@@ -1872,9 +1877,9 @@
     </row>
     <row r="22" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="5"/>
-      <c r="D22" s="113"/>
-      <c r="E22" s="114"/>
-      <c r="F22" s="118"/>
+      <c r="D22" s="68"/>
+      <c r="E22" s="69"/>
+      <c r="F22" s="73"/>
       <c r="G22" s="16" t="s">
         <v>80</v>
       </c>
@@ -1885,9 +1890,9 @@
     </row>
     <row r="23" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="5"/>
-      <c r="D23" s="113"/>
-      <c r="E23" s="114"/>
-      <c r="F23" s="118"/>
+      <c r="D23" s="68"/>
+      <c r="E23" s="69"/>
+      <c r="F23" s="73"/>
       <c r="G23" s="16" t="s">
         <v>81</v>
       </c>
@@ -1898,9 +1903,9 @@
     </row>
     <row r="24" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="5"/>
-      <c r="D24" s="113"/>
-      <c r="E24" s="114"/>
-      <c r="F24" s="118"/>
+      <c r="D24" s="68"/>
+      <c r="E24" s="69"/>
+      <c r="F24" s="73"/>
       <c r="G24" s="16" t="s">
         <v>82</v>
       </c>
@@ -1912,9 +1917,9 @@
     </row>
     <row r="25" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="5"/>
-      <c r="D25" s="113"/>
-      <c r="E25" s="114"/>
-      <c r="F25" s="118"/>
+      <c r="D25" s="68"/>
+      <c r="E25" s="69"/>
+      <c r="F25" s="73"/>
       <c r="G25" s="16" t="s">
         <v>83</v>
       </c>
@@ -1925,9 +1930,9 @@
     </row>
     <row r="26" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="5"/>
-      <c r="D26" s="113"/>
-      <c r="E26" s="114"/>
-      <c r="F26" s="118"/>
+      <c r="D26" s="68"/>
+      <c r="E26" s="69"/>
+      <c r="F26" s="73"/>
       <c r="G26" s="16" t="s">
         <v>84</v>
       </c>
@@ -1938,9 +1943,9 @@
     </row>
     <row r="27" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="5"/>
-      <c r="D27" s="113"/>
-      <c r="E27" s="114"/>
-      <c r="F27" s="118"/>
+      <c r="D27" s="68"/>
+      <c r="E27" s="69"/>
+      <c r="F27" s="73"/>
       <c r="G27" s="16" t="s">
         <v>85</v>
       </c>
@@ -1952,9 +1957,9 @@
     </row>
     <row r="28" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="5"/>
-      <c r="D28" s="113"/>
-      <c r="E28" s="114"/>
-      <c r="F28" s="118"/>
+      <c r="D28" s="68"/>
+      <c r="E28" s="69"/>
+      <c r="F28" s="73"/>
       <c r="G28" s="16" t="s">
         <v>86</v>
       </c>
@@ -1965,9 +1970,9 @@
     </row>
     <row r="29" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="5"/>
-      <c r="D29" s="113"/>
-      <c r="E29" s="114"/>
-      <c r="F29" s="118"/>
+      <c r="D29" s="68"/>
+      <c r="E29" s="69"/>
+      <c r="F29" s="73"/>
       <c r="G29" s="16" t="s">
         <v>87</v>
       </c>
@@ -1979,9 +1984,9 @@
     </row>
     <row r="30" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="5"/>
-      <c r="D30" s="113"/>
-      <c r="E30" s="114"/>
-      <c r="F30" s="118"/>
+      <c r="D30" s="68"/>
+      <c r="E30" s="69"/>
+      <c r="F30" s="73"/>
       <c r="G30" s="16" t="s">
         <v>88</v>
       </c>
@@ -1993,9 +1998,9 @@
     </row>
     <row r="31" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="5"/>
-      <c r="D31" s="113"/>
-      <c r="E31" s="114"/>
-      <c r="F31" s="118"/>
+      <c r="D31" s="68"/>
+      <c r="E31" s="69"/>
+      <c r="F31" s="73"/>
       <c r="G31" s="16" t="s">
         <v>89</v>
       </c>
@@ -2006,158 +2011,158 @@
     </row>
     <row r="32" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="5"/>
-      <c r="D32" s="113"/>
-      <c r="E32" s="114"/>
-      <c r="F32" s="118"/>
+      <c r="D32" s="68"/>
+      <c r="E32" s="69"/>
+      <c r="F32" s="73"/>
       <c r="G32" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="H32" s="115" t="s">
+      <c r="H32" s="70" t="s">
         <v>32</v>
       </c>
-      <c r="I32" s="116"/>
+      <c r="I32" s="71"/>
     </row>
     <row r="33" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="5"/>
-      <c r="D33" s="113"/>
-      <c r="E33" s="114"/>
-      <c r="F33" s="118"/>
+      <c r="D33" s="68"/>
+      <c r="E33" s="69"/>
+      <c r="F33" s="73"/>
       <c r="G33" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="H33" s="115" t="s">
+      <c r="H33" s="70" t="s">
         <v>33</v>
       </c>
-      <c r="I33" s="116"/>
+      <c r="I33" s="71"/>
     </row>
     <row r="34" spans="2:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="5"/>
-      <c r="D34" s="97" t="s">
+      <c r="D34" s="74" t="s">
         <v>34</v>
       </c>
-      <c r="E34" s="97"/>
+      <c r="E34" s="74"/>
       <c r="F34" s="20">
         <v>16038</v>
       </c>
-      <c r="G34" s="98"/>
-      <c r="H34" s="99"/>
-      <c r="I34" s="100"/>
+      <c r="G34" s="75"/>
+      <c r="H34" s="76"/>
+      <c r="I34" s="77"/>
     </row>
     <row r="35" spans="2:10" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="5"/>
-      <c r="D35" s="101" t="s">
+      <c r="D35" s="78" t="s">
         <v>35</v>
       </c>
-      <c r="E35" s="102"/>
-      <c r="F35" s="105">
+      <c r="E35" s="79"/>
+      <c r="F35" s="82">
         <f>SUM(G35:G44)</f>
         <v>-97</v>
       </c>
       <c r="G35" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="H35" s="103" t="s">
+      <c r="H35" s="80" t="s">
         <v>36</v>
       </c>
-      <c r="I35" s="104"/>
+      <c r="I35" s="81"/>
     </row>
     <row r="36" spans="2:10" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="5"/>
-      <c r="D36" s="101"/>
-      <c r="E36" s="102"/>
-      <c r="F36" s="105"/>
+      <c r="D36" s="78"/>
+      <c r="E36" s="79"/>
+      <c r="F36" s="82"/>
       <c r="G36" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="H36" s="103" t="s">
+      <c r="H36" s="80" t="s">
         <v>37</v>
       </c>
-      <c r="I36" s="104"/>
+      <c r="I36" s="81"/>
     </row>
     <row r="37" spans="2:10" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="5"/>
-      <c r="D37" s="101"/>
-      <c r="E37" s="102"/>
-      <c r="F37" s="105"/>
+      <c r="D37" s="78"/>
+      <c r="E37" s="79"/>
+      <c r="F37" s="82"/>
       <c r="G37" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="H37" s="103" t="s">
+      <c r="H37" s="80" t="s">
         <v>38</v>
       </c>
-      <c r="I37" s="104"/>
+      <c r="I37" s="81"/>
     </row>
     <row r="38" spans="2:10" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="5"/>
-      <c r="D38" s="101"/>
-      <c r="E38" s="102"/>
-      <c r="F38" s="105"/>
+      <c r="D38" s="78"/>
+      <c r="E38" s="79"/>
+      <c r="F38" s="82"/>
       <c r="G38" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="H38" s="103" t="s">
+      <c r="H38" s="80" t="s">
         <v>39</v>
       </c>
-      <c r="I38" s="104"/>
+      <c r="I38" s="81"/>
     </row>
     <row r="39" spans="2:10" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="5"/>
-      <c r="D39" s="101"/>
-      <c r="E39" s="102"/>
-      <c r="F39" s="105"/>
+      <c r="D39" s="78"/>
+      <c r="E39" s="79"/>
+      <c r="F39" s="82"/>
       <c r="G39" s="21">
         <v>-97</v>
       </c>
-      <c r="H39" s="103" t="s">
+      <c r="H39" s="80" t="s">
         <v>40</v>
       </c>
-      <c r="I39" s="104"/>
+      <c r="I39" s="81"/>
     </row>
     <row r="40" spans="2:10" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="5"/>
-      <c r="D40" s="101"/>
-      <c r="E40" s="102"/>
-      <c r="F40" s="105"/>
+      <c r="D40" s="78"/>
+      <c r="E40" s="79"/>
+      <c r="F40" s="82"/>
       <c r="G40" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="H40" s="103" t="s">
+      <c r="H40" s="80" t="s">
         <v>41</v>
       </c>
-      <c r="I40" s="104"/>
+      <c r="I40" s="81"/>
     </row>
     <row r="41" spans="2:10" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="5"/>
-      <c r="D41" s="101"/>
-      <c r="E41" s="102"/>
-      <c r="F41" s="105"/>
+      <c r="D41" s="78"/>
+      <c r="E41" s="79"/>
+      <c r="F41" s="82"/>
       <c r="G41" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="H41" s="103" t="s">
+      <c r="H41" s="80" t="s">
         <v>42</v>
       </c>
-      <c r="I41" s="104"/>
+      <c r="I41" s="81"/>
     </row>
     <row r="42" spans="2:10" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="5"/>
-      <c r="D42" s="101"/>
-      <c r="E42" s="102"/>
-      <c r="F42" s="105"/>
+      <c r="D42" s="78"/>
+      <c r="E42" s="79"/>
+      <c r="F42" s="82"/>
       <c r="G42" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="H42" s="103" t="s">
+      <c r="H42" s="80" t="s">
         <v>43</v>
       </c>
-      <c r="I42" s="104"/>
+      <c r="I42" s="81"/>
       <c r="J42" s="19"/>
     </row>
     <row r="43" spans="2:10" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="5"/>
-      <c r="D43" s="101"/>
-      <c r="E43" s="102"/>
-      <c r="F43" s="105"/>
+      <c r="D43" s="78"/>
+      <c r="E43" s="79"/>
+      <c r="F43" s="82"/>
       <c r="G43" s="21" t="s">
         <v>99</v>
       </c>
@@ -2169,23 +2174,23 @@
     </row>
     <row r="44" spans="2:10" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="5"/>
-      <c r="D44" s="101"/>
-      <c r="E44" s="102"/>
-      <c r="F44" s="105"/>
+      <c r="D44" s="78"/>
+      <c r="E44" s="79"/>
+      <c r="F44" s="82"/>
       <c r="G44" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="H44" s="106" t="s">
+      <c r="H44" s="83" t="s">
         <v>45</v>
       </c>
-      <c r="I44" s="107"/>
+      <c r="I44" s="84"/>
     </row>
     <row r="45" spans="2:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="5"/>
-      <c r="D45" s="92" t="s">
+      <c r="D45" s="85" t="s">
         <v>46</v>
       </c>
-      <c r="E45" s="92"/>
+      <c r="E45" s="85"/>
       <c r="F45" s="24">
         <f>SUM(F34:F44)</f>
         <v>15941</v>
@@ -2194,10 +2199,10 @@
     </row>
     <row r="46" spans="2:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="5"/>
-      <c r="D46" s="84" t="s">
+      <c r="D46" s="86" t="s">
         <v>47</v>
       </c>
-      <c r="E46" s="84"/>
+      <c r="E46" s="86"/>
       <c r="F46" s="25">
         <f>F13-F45</f>
         <v>-15941</v>
@@ -2235,16 +2240,16 @@
       <c r="I49" s="12"/>
     </row>
     <row r="50" spans="2:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="93" t="s">
+      <c r="B50" s="87" t="s">
         <v>48</v>
       </c>
-      <c r="C50" s="94"/>
-      <c r="D50" s="94"/>
-      <c r="E50" s="94"/>
-      <c r="F50" s="94"/>
-      <c r="G50" s="94"/>
-      <c r="H50" s="94"/>
-      <c r="I50" s="95"/>
+      <c r="C50" s="88"/>
+      <c r="D50" s="88"/>
+      <c r="E50" s="88"/>
+      <c r="F50" s="88"/>
+      <c r="G50" s="88"/>
+      <c r="H50" s="88"/>
+      <c r="I50" s="89"/>
     </row>
     <row r="51" spans="2:9" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="2"/>
@@ -2258,11 +2263,11 @@
     </row>
     <row r="52" spans="2:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="5"/>
-      <c r="D52" s="96" t="s">
+      <c r="D52" s="90" t="s">
         <v>49</v>
       </c>
-      <c r="E52" s="96"/>
-      <c r="F52" s="96"/>
+      <c r="E52" s="90"/>
+      <c r="F52" s="90"/>
       <c r="G52" s="37" t="s">
         <v>50</v>
       </c>
@@ -2270,10 +2275,10 @@
     </row>
     <row r="53" spans="2:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="5"/>
-      <c r="D53" s="84">
+      <c r="D53" s="86">
         <v>171014</v>
       </c>
-      <c r="E53" s="84"/>
+      <c r="E53" s="86"/>
       <c r="F53" s="38" t="s">
         <v>101</v>
       </c>
@@ -2285,10 +2290,10 @@
     </row>
     <row r="54" spans="2:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="5"/>
-      <c r="D54" s="84">
+      <c r="D54" s="86">
         <v>170516</v>
       </c>
-      <c r="E54" s="84"/>
+      <c r="E54" s="86"/>
       <c r="F54" s="38" t="s">
         <v>102</v>
       </c>
@@ -2300,10 +2305,10 @@
     </row>
     <row r="55" spans="2:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="5"/>
-      <c r="D55" s="84" t="s">
+      <c r="D55" s="86" t="s">
         <v>51</v>
       </c>
-      <c r="E55" s="84"/>
+      <c r="E55" s="86"/>
       <c r="F55" s="42" t="s">
         <v>103</v>
       </c>
@@ -2316,10 +2321,10 @@
     <row r="56" spans="2:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="28"/>
       <c r="C56" s="29"/>
-      <c r="D56" s="85" t="s">
+      <c r="D56" s="91" t="s">
         <v>52</v>
       </c>
-      <c r="E56" s="85"/>
+      <c r="E56" s="91"/>
       <c r="F56" s="44">
         <f>SUM(F53:F55)</f>
         <v>0</v>
@@ -2336,16 +2341,16 @@
       <c r="I57" s="12"/>
     </row>
     <row r="58" spans="2:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="86" t="s">
+      <c r="B58" s="60" t="s">
         <v>53</v>
       </c>
-      <c r="C58" s="87"/>
-      <c r="D58" s="87"/>
-      <c r="E58" s="87"/>
-      <c r="F58" s="87"/>
-      <c r="G58" s="87"/>
-      <c r="H58" s="87"/>
-      <c r="I58" s="88"/>
+      <c r="C58" s="61"/>
+      <c r="D58" s="61"/>
+      <c r="E58" s="61"/>
+      <c r="F58" s="61"/>
+      <c r="G58" s="61"/>
+      <c r="H58" s="61"/>
+      <c r="I58" s="62"/>
     </row>
     <row r="59" spans="2:9" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="2"/>
@@ -2359,11 +2364,11 @@
     </row>
     <row r="60" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="5"/>
-      <c r="D60" s="89" t="s">
+      <c r="D60" s="58" t="s">
         <v>54</v>
       </c>
-      <c r="E60" s="90"/>
-      <c r="F60" s="91"/>
+      <c r="E60" s="92"/>
+      <c r="F60" s="59"/>
       <c r="G60" s="36" t="s">
         <v>11</v>
       </c>
@@ -2371,31 +2376,31 @@
     </row>
     <row r="61" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="5"/>
-      <c r="D61" s="70" t="s">
+      <c r="D61" s="93" t="s">
         <v>55</v>
       </c>
-      <c r="E61" s="71"/>
-      <c r="F61" s="72"/>
-      <c r="G61" s="76">
+      <c r="E61" s="94"/>
+      <c r="F61" s="95"/>
+      <c r="G61" s="99">
         <v>8929</v>
       </c>
       <c r="I61" s="12"/>
     </row>
     <row r="62" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="5"/>
-      <c r="D62" s="73"/>
-      <c r="E62" s="74"/>
-      <c r="F62" s="75"/>
-      <c r="G62" s="77"/>
+      <c r="D62" s="96"/>
+      <c r="E62" s="97"/>
+      <c r="F62" s="98"/>
+      <c r="G62" s="100"/>
       <c r="I62" s="12"/>
     </row>
     <row r="63" spans="2:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="5"/>
-      <c r="D63" s="78" t="s">
+      <c r="D63" s="101" t="s">
         <v>56</v>
       </c>
-      <c r="E63" s="79"/>
-      <c r="F63" s="80"/>
+      <c r="E63" s="102"/>
+      <c r="F63" s="103"/>
       <c r="G63" s="47">
         <v>8103</v>
       </c>
@@ -2404,40 +2409,40 @@
     </row>
     <row r="64" spans="2:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="5"/>
-      <c r="D64" s="81" t="s">
+      <c r="D64" s="104" t="s">
         <v>57</v>
       </c>
-      <c r="E64" s="82"/>
-      <c r="F64" s="83"/>
+      <c r="E64" s="105"/>
+      <c r="F64" s="106"/>
       <c r="G64" s="49">
         <f>G61-G63</f>
         <v>826</v>
       </c>
-      <c r="H64" s="64" t="s">
+      <c r="H64" s="107" t="s">
         <v>58</v>
       </c>
-      <c r="I64" s="65"/>
+      <c r="I64" s="108"/>
     </row>
     <row r="65" spans="2:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="5"/>
-      <c r="D65" s="63" t="s">
+      <c r="D65" s="109" t="s">
         <v>59</v>
       </c>
-      <c r="E65" s="63"/>
-      <c r="F65" s="63"/>
+      <c r="E65" s="109"/>
+      <c r="F65" s="109"/>
       <c r="G65" s="38"/>
-      <c r="H65" s="64" t="s">
+      <c r="H65" s="107" t="s">
         <v>60</v>
       </c>
-      <c r="I65" s="65"/>
+      <c r="I65" s="108"/>
     </row>
     <row r="66" spans="2:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="5"/>
-      <c r="D66" s="63" t="s">
+      <c r="D66" s="109" t="s">
         <v>61</v>
       </c>
-      <c r="E66" s="63"/>
-      <c r="F66" s="63"/>
+      <c r="E66" s="109"/>
+      <c r="F66" s="109"/>
       <c r="G66" s="38" t="s">
         <v>104</v>
       </c>
@@ -2461,56 +2466,56 @@
     </row>
     <row r="69" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B69" s="5"/>
-      <c r="D69" s="66" t="s">
+      <c r="D69" s="110" t="s">
         <v>62</v>
       </c>
-      <c r="E69" s="66"/>
-      <c r="F69" s="66"/>
-      <c r="G69" s="66"/>
-      <c r="H69" s="66"/>
-      <c r="I69" s="67"/>
+      <c r="E69" s="110"/>
+      <c r="F69" s="110"/>
+      <c r="G69" s="110"/>
+      <c r="H69" s="110"/>
+      <c r="I69" s="111"/>
     </row>
     <row r="70" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B70" s="5"/>
-      <c r="D70" s="68"/>
-      <c r="E70" s="68"/>
-      <c r="F70" s="68"/>
-      <c r="G70" s="68"/>
-      <c r="H70" s="68"/>
-      <c r="I70" s="69"/>
+      <c r="D70" s="112"/>
+      <c r="E70" s="112"/>
+      <c r="F70" s="112"/>
+      <c r="G70" s="112"/>
+      <c r="H70" s="112"/>
+      <c r="I70" s="113"/>
     </row>
     <row r="71" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B71" s="5"/>
-      <c r="D71" s="56" t="s">
+      <c r="D71" s="115" t="s">
         <v>63</v>
       </c>
-      <c r="E71" s="56"/>
-      <c r="F71" s="56"/>
-      <c r="G71" s="56"/>
-      <c r="H71" s="56"/>
-      <c r="I71" s="57"/>
+      <c r="E71" s="115"/>
+      <c r="F71" s="115"/>
+      <c r="G71" s="115"/>
+      <c r="H71" s="115"/>
+      <c r="I71" s="116"/>
     </row>
     <row r="72" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B72" s="5"/>
-      <c r="D72" s="58" t="s">
+      <c r="D72" s="117" t="s">
         <v>64</v>
       </c>
-      <c r="E72" s="58"/>
-      <c r="F72" s="58"/>
-      <c r="G72" s="58"/>
-      <c r="H72" s="58"/>
-      <c r="I72" s="59"/>
+      <c r="E72" s="117"/>
+      <c r="F72" s="117"/>
+      <c r="G72" s="117"/>
+      <c r="H72" s="117"/>
+      <c r="I72" s="118"/>
     </row>
     <row r="73" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B73" s="5"/>
-      <c r="D73" s="58" t="s">
+      <c r="D73" s="117" t="s">
         <v>65</v>
       </c>
-      <c r="E73" s="58"/>
-      <c r="F73" s="58"/>
-      <c r="G73" s="58"/>
-      <c r="H73" s="58"/>
-      <c r="I73" s="59"/>
+      <c r="E73" s="117"/>
+      <c r="F73" s="117"/>
+      <c r="G73" s="117"/>
+      <c r="H73" s="117"/>
+      <c r="I73" s="118"/>
     </row>
     <row r="74" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B74" s="5"/>
@@ -2518,14 +2523,14 @@
     </row>
     <row r="75" spans="2:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B75" s="5"/>
-      <c r="D75" s="60" t="s">
+      <c r="D75" s="119" t="s">
         <v>66</v>
       </c>
-      <c r="E75" s="60"/>
-      <c r="F75" s="60"/>
-      <c r="G75" s="60"/>
-      <c r="H75" s="60"/>
-      <c r="I75" s="61"/>
+      <c r="E75" s="119"/>
+      <c r="F75" s="119"/>
+      <c r="G75" s="119"/>
+      <c r="H75" s="119"/>
+      <c r="I75" s="120"/>
     </row>
     <row r="76" spans="2:9" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" s="5"/>
@@ -2533,26 +2538,26 @@
     </row>
     <row r="77" spans="2:9" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B77" s="53"/>
-      <c r="D77" s="62" t="s">
+      <c r="D77" s="121" t="s">
         <v>7</v>
       </c>
-      <c r="E77" s="62"/>
-      <c r="G77" s="62" t="s">
+      <c r="E77" s="121"/>
+      <c r="G77" s="121" t="s">
         <v>8</v>
       </c>
-      <c r="H77" s="62"/>
+      <c r="H77" s="121"/>
       <c r="I77" s="54"/>
     </row>
     <row r="78" spans="2:9" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B78" s="5"/>
-      <c r="D78" s="55" t="s">
+      <c r="D78" s="114" t="s">
         <v>3</v>
       </c>
-      <c r="E78" s="55"/>
-      <c r="G78" s="55" t="s">
+      <c r="E78" s="114"/>
+      <c r="G78" s="114" t="s">
         <v>67</v>
       </c>
-      <c r="H78" s="55"/>
+      <c r="H78" s="114"/>
       <c r="I78" s="12"/>
     </row>
     <row r="79" spans="2:9" x14ac:dyDescent="0.25">
@@ -2585,21 +2590,34 @@
     </row>
   </sheetData>
   <mergeCells count="56">
-    <mergeCell ref="E2:I2"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="B10:I10"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="D13:E33"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="F13:F33"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="D78:E78"/>
+    <mergeCell ref="G78:H78"/>
+    <mergeCell ref="D71:I71"/>
+    <mergeCell ref="D72:I72"/>
+    <mergeCell ref="D73:I73"/>
+    <mergeCell ref="D75:I75"/>
+    <mergeCell ref="D77:E77"/>
+    <mergeCell ref="G77:H77"/>
+    <mergeCell ref="D65:F65"/>
+    <mergeCell ref="H65:I65"/>
+    <mergeCell ref="D66:F66"/>
+    <mergeCell ref="D69:I69"/>
+    <mergeCell ref="D70:I70"/>
+    <mergeCell ref="D61:F62"/>
+    <mergeCell ref="G61:G62"/>
+    <mergeCell ref="D63:F63"/>
+    <mergeCell ref="D64:F64"/>
+    <mergeCell ref="H64:I64"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="B58:I58"/>
+    <mergeCell ref="D60:F60"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="B50:I50"/>
+    <mergeCell ref="D52:F52"/>
+    <mergeCell ref="D53:E53"/>
     <mergeCell ref="D34:E34"/>
     <mergeCell ref="G34:I34"/>
     <mergeCell ref="D35:E44"/>
@@ -2613,34 +2631,21 @@
     <mergeCell ref="H41:I41"/>
     <mergeCell ref="H42:I42"/>
     <mergeCell ref="H44:I44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="B50:I50"/>
-    <mergeCell ref="D52:F52"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="B58:I58"/>
-    <mergeCell ref="D60:F60"/>
-    <mergeCell ref="D61:F62"/>
-    <mergeCell ref="G61:G62"/>
-    <mergeCell ref="D63:F63"/>
-    <mergeCell ref="D64:F64"/>
-    <mergeCell ref="H64:I64"/>
-    <mergeCell ref="D65:F65"/>
-    <mergeCell ref="H65:I65"/>
-    <mergeCell ref="D66:F66"/>
-    <mergeCell ref="D69:I69"/>
-    <mergeCell ref="D70:I70"/>
-    <mergeCell ref="D78:E78"/>
-    <mergeCell ref="G78:H78"/>
-    <mergeCell ref="D71:I71"/>
-    <mergeCell ref="D72:I72"/>
-    <mergeCell ref="D73:I73"/>
-    <mergeCell ref="D75:I75"/>
-    <mergeCell ref="D77:E77"/>
-    <mergeCell ref="G77:H77"/>
+    <mergeCell ref="B10:I10"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="D13:E33"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="F13:F33"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="E2:I2"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="G6:H6"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.15748031496062992" bottom="0.15748031496062992" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>